<commit_message>
2022 January 8 - Minor fixes in modeling code.
</commit_message>
<xml_diff>
--- a/cost_function.xlsx
+++ b/cost_function.xlsx
@@ -45,13 +45,13 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>TN *( +2898)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> FP * (-2898)</t>
-  </si>
-  <si>
     <t>FN * (-216428)</t>
+  </si>
+  <si>
+    <t>TN *( +28983)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FP * (-28983)</t>
   </si>
 </sst>
 </file>
@@ -351,40 +351,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -684,7 +684,7 @@
   <dimension ref="B5:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -718,88 +718,88 @@
     <row r="7" spans="2:12" ht="30" customHeight="1">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E7" s="12"/>
+      <c r="E7" s="16"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="I7" s="3"/>
       <c r="J7" s="4"/>
-      <c r="K7" s="11" t="s">
+      <c r="K7" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="L7" s="12"/>
+      <c r="L7" s="16"/>
     </row>
     <row r="8" spans="2:12" ht="30" customHeight="1">
       <c r="B8" s="5"/>
       <c r="C8" s="6"/>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="10" t="s">
         <v>3</v>
       </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="I8" s="5"/>
       <c r="J8" s="6"/>
-      <c r="K8" s="13" t="s">
+      <c r="K8" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:12" ht="34.5" customHeight="1">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="D9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="12" t="s">
         <v>7</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="K9" s="15" t="s">
+      <c r="K9" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9" s="12" t="s">
         <v>9</v>
-      </c>
-      <c r="L9" s="16" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="2:12" ht="36" customHeight="1">
-      <c r="B10" s="9"/>
-      <c r="C10" s="10" t="s">
+      <c r="B10" s="18"/>
+      <c r="C10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="17" t="s">
+      <c r="D10" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="14" t="s">
         <v>4</v>
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10" t="s">
+      <c r="I10" s="18"/>
+      <c r="J10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="K10" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="L10" s="18" t="s">
+      <c r="K10" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="L10" s="14" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>